<commit_message>
Update Visualizacion cubos Hiriart Corales.xlsx
</commit_message>
<xml_diff>
--- a/Visualizacion cubos Hiriart Corales.xlsx
+++ b/Visualizacion cubos Hiriart Corales.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code-UDLA\BDIII\Proyecto-BI-Hiriart-Corales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A16775C0-1E7B-4C92-AC8D-93FDA9EC3266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{439A744B-508C-4D01-9A26-9D6A5EFBF928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="2640" yWindow="1635" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="tmpB560" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="130" r:id="rId2"/>
+    <pivotCache cacheId="163" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -36,13 +36,14 @@
   <metadataTypes count="1">
     <metadataType name="XLMDX" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <metadataStrings count="4">
+  <metadataStrings count="5">
     <s v="DIEGOHL\SQLDEV EstadSeguridadHC_OLAP"/>
-    <s v="{[Localidad Dim].[Provincia].&amp;[GUAYAS]}"/>
-    <s v="{[Tiempo Dim].[Anio].&amp;[2019],[Tiempo Dim].[Anio].&amp;[2020]}"/>
-    <s v="{[Tiempo Dim].[Trimestre].&amp;[2]}"/>
+    <s v="{[Tiempo Dim].[Trimestre].[All]}"/>
+    <s v="{[Tiempo Dim].[Anio].&amp;[2022]}"/>
+    <s v="{[Localidad Dim].[Provincia].[All]}"/>
+    <s v="{[Tiempo Dim].[Mes].&amp;[3]}"/>
   </metadataStrings>
-  <mdxMetadata count="3">
+  <mdxMetadata count="4">
     <mdx n="0" f="s">
       <ms ns="1" c="0"/>
     </mdx>
@@ -52,8 +53,11 @@
     <mdx n="0" f="s">
       <ms ns="3" c="0"/>
     </mdx>
+    <mdx n="0" f="s">
+      <ms ns="4" c="0"/>
+    </mdx>
   </mdxMetadata>
-  <valueMetadata count="3">
+  <valueMetadata count="4">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -63,12 +67,15 @@
     <bk>
       <rc t="1" v="2"/>
     </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Crimenes Fact Count</t>
   </si>
@@ -109,10 +116,10 @@
     <t>OTROS</t>
   </si>
   <si>
-    <t>GUAYAS</t>
+    <t>2022</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
   <si>
     <t>Provincia</t>
@@ -121,10 +128,13 @@
     <t>Anio</t>
   </si>
   <si>
-    <t>(Multiple Items)</t>
+    <t>Trimestre</t>
   </si>
   <si>
-    <t>Trimestre</t>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Mes</t>
   </si>
 </sst>
 </file>
@@ -841,9 +851,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>tmpB560!$A$8:$A$26</c:f>
+              <c:f>tmpB560!$A$8:$A$25</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>ARMA BLANCA</c:v>
@@ -867,24 +877,21 @@
                     <c:v>ARMA DE FUEGO</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>CONSTRICTORA</c:v>
+                    <c:v>OTROS</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>ARMA BLANCA</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>ARMA CONTUNDENTE</c:v>
+                    <c:v>ARMA DE FUEGO</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>ARMA DE FUEGO</c:v>
+                    <c:v>CONSTRICTORA</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>CONSTRICTORA</c:v>
+                    <c:v>OTROS</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>OTROS</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
                     <c:v>ARMA DE FUEGO</c:v>
                   </c:pt>
                 </c:lvl>
@@ -898,7 +905,7 @@
                   <c:pt idx="8">
                     <c:v>HOMICIDIO</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="12">
                     <c:v>SICARIATO</c:v>
                   </c:pt>
                 </c:lvl>
@@ -907,58 +914,55 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>tmpB560!$B$8:$B$26</c:f>
+              <c:f>tmpB560!$B$8:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6E07-4F0D-BB03-6D825E75CA66}"/>
+              <c16:uniqueId val="{00000007-6E07-4F0D-BB03-6D825E75CA66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -988,9 +992,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>tmpB560!$A$8:$A$26</c:f>
+              <c:f>tmpB560!$A$8:$A$25</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>ARMA BLANCA</c:v>
@@ -1014,24 +1018,21 @@
                     <c:v>ARMA DE FUEGO</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>CONSTRICTORA</c:v>
+                    <c:v>OTROS</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>ARMA BLANCA</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>ARMA CONTUNDENTE</c:v>
+                    <c:v>ARMA DE FUEGO</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>ARMA DE FUEGO</c:v>
+                    <c:v>CONSTRICTORA</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>CONSTRICTORA</c:v>
+                    <c:v>OTROS</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>OTROS</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
                     <c:v>ARMA DE FUEGO</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1045,7 +1046,7 @@
                   <c:pt idx="8">
                     <c:v>HOMICIDIO</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="12">
                     <c:v>SICARIATO</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1054,58 +1055,55 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>tmpB560!$C$8:$C$26</c:f>
+              <c:f>tmpB560!$C$8:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6E07-4F0D-BB03-6D825E75CA66}"/>
+              <c16:uniqueId val="{00000008-6E07-4F0D-BB03-6D825E75CA66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1912,9 +1910,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Diego HL" refreshedDate="44747.847548032405" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Diego HL" refreshedDate="44747.904356250001" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="7">
+  <cacheFields count="8">
     <cacheField name="[Clasificacion Dim].[Nombre].[Nombre]" caption="Nombre" numFmtId="0" hierarchy="2" level="1">
       <sharedItems count="4">
         <s v="[Clasificacion Dim].[Nombre].&amp;[ASESINATO]" c="ASESINATO"/>
@@ -1933,21 +1931,21 @@
       </sharedItems>
     </cacheField>
     <cacheField name="[Localidad Dim].[Provincia].[Provincia]" caption="Provincia" numFmtId="0" hierarchy="11" level="1">
-      <sharedItems count="1">
-        <s v="[Localidad Dim].[Provincia].&amp;[GUAYAS]" c="GUAYAS"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
     <cacheField name="[Tiempo Dim].[Anio].[Anio]" caption="Anio" numFmtId="0" hierarchy="13" level="1">
-      <sharedItems count="2">
-        <s v="[Tiempo Dim].[Anio].&amp;[2019]" c="2019"/>
-        <s v="[Tiempo Dim].[Anio].&amp;[2020]" c="2020"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
     <cacheField name="[Tiempo Dim].[Trimestre].[Trimestre]" caption="Trimestre" numFmtId="0" hierarchy="18" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
     <cacheField name="[Measures].[Crimenes Fact Count]" caption="Crimenes Fact Count" numFmtId="0" hierarchy="20" level="32767"/>
     <cacheField name="[Measures].[Afectados]" caption="Afectados" numFmtId="0" hierarchy="19" level="32767"/>
+    <cacheField name="[Tiempo Dim].[Mes].[Mes]" caption="Mes" numFmtId="0" hierarchy="14" level="1">
+      <sharedItems count="1">
+        <s v="[Tiempo Dim].[Mes].&amp;[4]" c="4"/>
+      </sharedItems>
+    </cacheField>
   </cacheFields>
   <cacheHierarchies count="21">
     <cacheHierarchy uniqueName="[Clasificacion Dim].[Clasificacion ID]" caption="Clasificacion ID" attribute="1" defaultMemberUniqueName="[Clasificacion Dim].[Clasificacion ID].[All]" allUniqueName="[Clasificacion Dim].[Clasificacion ID].[All]" dimensionUniqueName="[Clasificacion Dim]" displayFolder="" count="0" unbalanced="0"/>
@@ -1984,7 +1982,12 @@
         <fieldUsage x="3"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Tiempo Dim].[Mes]" caption="Mes" attribute="1" defaultMemberUniqueName="[Tiempo Dim].[Mes].[All]" allUniqueName="[Tiempo Dim].[Mes].[All]" dimensionUniqueName="[Tiempo Dim]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Tiempo Dim].[Mes]" caption="Mes" attribute="1" defaultMemberUniqueName="[Tiempo Dim].[Mes].[All]" allUniqueName="[Tiempo Dim].[Mes].[All]" dimensionUniqueName="[Tiempo Dim]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="7"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Tiempo Dim].[Mes Anio]" caption="Mes Anio" attribute="1" defaultMemberUniqueName="[Tiempo Dim].[Mes Anio].[All]" allUniqueName="[Tiempo Dim].[Mes Anio].[All]" dimensionUniqueName="[Tiempo Dim]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Tiempo Dim].[Periodo]" caption="Periodo" attribute="1" defaultMemberUniqueName="[Tiempo Dim].[Periodo].[All]" allUniqueName="[Tiempo Dim].[Periodo].[All]" dimensionUniqueName="[Tiempo Dim]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Tiempo Dim].[Tiempo Key]" caption="Tiempo Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tiempo Dim].[Tiempo Key].[All]" allUniqueName="[Tiempo Dim].[Tiempo Key].[All]" dimensionUniqueName="[Tiempo Dim]" displayFolder="" count="0" unbalanced="0"/>
@@ -2031,9 +2034,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="130" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
-  <location ref="A7:C26" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="163" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+  <location ref="A7:C25" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="8">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
       <items count="4">
         <item x="0"/>
@@ -2051,26 +2054,22 @@
         <item x="4"/>
       </items>
     </pivotField>
-    <pivotField axis="axisPage" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="1">
-        <item s="1" x="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="2">
-        <item s="1" x="0"/>
-        <item s="1" x="1"/>
-      </items>
-    </pivotField>
+    <pivotField axis="axisPage" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1"/>
+    <pivotField axis="axisPage" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1"/>
     <pivotField axis="axisPage" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisPage" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="2">
     <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="19">
+  <rowItems count="18">
     <i>
       <x/>
     </i>
@@ -2099,16 +2098,13 @@
       <x v="2"/>
     </i>
     <i r="1">
-      <x v="3"/>
+      <x v="4"/>
     </i>
     <i>
       <x v="2"/>
     </i>
     <i r="1">
       <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
     </i>
     <i r="1">
       <x v="2"/>
@@ -2140,10 +2136,11 @@
       <x v="1"/>
     </i>
   </colItems>
-  <pageFields count="3">
-    <pageField fld="2" hier="11" name="[Localidad Dim].[Provincia].&amp;[GUAYAS]" cap="GUAYAS"/>
-    <pageField fld="3" hier="13" name="[Tiempo Dim].[Anio].&amp;[2019]" cap="2019"/>
-    <pageField fld="4" hier="18" name="[Tiempo Dim].[Trimestre].&amp;[2]" cap="2"/>
+  <pageFields count="4">
+    <pageField fld="2" hier="11" name="[Localidad Dim].[Provincia].[All]" cap="All"/>
+    <pageField fld="3" hier="13" name="[Tiempo Dim].[Anio].&amp;[2022]" cap="2022"/>
+    <pageField fld="4" hier="18" name="[Tiempo Dim].[Trimestre].[All]" cap="All"/>
+    <pageField fld="7" hier="14" name="[Tiempo Dim].[Mes].&amp;[3]" cap="3"/>
   </pageFields>
   <dataFields count="2">
     <dataField fld="5" baseField="0" baseItem="0"/>
@@ -2183,16 +2180,20 @@
     <pivotHierarchy/>
     <pivotHierarchy multipleItemSelectionAllowed="1"/>
     <pivotHierarchy/>
-    <pivotHierarchy multipleItemSelectionAllowed="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1">
+      <members count="1" level="1">
+        <member name="[Tiempo Dim].[Anio].&amp;[2022]"/>
+      </members>
+    </pivotHierarchy>
+    <pivotHierarchy multipleItemSelectionAllowed="1">
+      <members count="1" level="1">
+        <member name="[Tiempo Dim].[Mes].&amp;[3]"/>
+      </members>
+    </pivotHierarchy>
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy multipleItemSelectionAllowed="1">
-      <members count="1" level="1">
-        <member name="[Tiempo Dim].[Trimestre].&amp;[2]"/>
-      </members>
-    </pivotHierarchy>
+    <pivotHierarchy multipleItemSelectionAllowed="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
   </pivotHierarchies>
@@ -2512,10 +2513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C26"/>
+  <dimension ref="A2:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,27 +2526,35 @@
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s" vm="3">
+        <v>18</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s" vm="1">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" vm="2">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s" vm="2">
         <v>17</v>
+      </c>
+      <c r="B4" t="s" vm="1">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s" vm="3">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s" vm="4">
         <v>14</v>
       </c>
     </row>
@@ -2572,10 +2581,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2583,10 +2592,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2594,10 +2603,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="C11" s="1">
-        <v>120</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2605,10 +2614,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2616,10 +2625,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2634,10 +2643,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2653,13 +2662,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2674,37 +2683,37 @@
         <v>8</v>
       </c>
       <c r="B19" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1">
         <v>2</v>
@@ -2714,43 +2723,32 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
         <v>6</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>10</v>
+      <c r="A25" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="1">
-        <v>119</v>
-      </c>
-      <c r="C26" s="1">
-        <v>187</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>